<commit_message>
Added transport, commercial and industrial demands Added factor for energy losses Merged all regions for demand and supply
</commit_message>
<xml_diff>
--- a/storageoptim/storageoptions2.xlsx
+++ b/storageoptim/storageoptions2.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,10 +417,10 @@
         <v>100000</v>
       </c>
       <c r="C2">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="D2">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="E2">
         <v>0.8</v>
@@ -463,13 +463,13 @@
         <v>5000</v>
       </c>
       <c r="C4">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="D4">
         <v>0.95</v>
       </c>
       <c r="E4">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F4">
         <v>0.5</v>

</xml_diff>